<commit_message>
added examples for versioned access
</commit_message>
<xml_diff>
--- a/CapStatement/temp_source_spreadsheets/carin-bb-server.xlsx
+++ b/CapStatement/temp_source_spreadsheets/carin-bb-server.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skravitz/git-alt/MyNotebooks/CapStatement/temp_source_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFE751C-6046-384F-8194-041A5CD84B74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60018A8-F577-CF40-924F-DDC51BDCB072}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="64520" windowHeight="25180" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4280" yWindow="2780" windowWidth="64520" windowHeight="25180" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet name="sp_combos" sheetId="8" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">sp_combos!$B$1:$B$77</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">sp_combos!$B$1:$B$76</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">sps!$A$1:$AB$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="184">
   <si>
     <t>Element</t>
   </si>
@@ -188,15 +188,9 @@
     <t>resolves</t>
   </si>
   <si>
-    <t>AllergyIntolerance</t>
-  </si>
-  <si>
     <t>Patient</t>
   </si>
   <si>
-    <t>Encounter</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -347,9 +341,6 @@
     <t>types</t>
   </si>
   <si>
-    <t>Condition</t>
-  </si>
-  <si>
     <t>category</t>
   </si>
   <si>
@@ -359,45 +350,12 @@
     <t>index</t>
   </si>
   <si>
-    <t>!Encounter</t>
-  </si>
-  <si>
-    <t>!Questionnaire</t>
-  </si>
-  <si>
-    <t>Immunization</t>
-  </si>
-  <si>
     <t>rel_url</t>
   </si>
   <si>
     <t>!EXAMPLE PATIENT SEARCH</t>
   </si>
   <si>
-    <t>DocumentReference</t>
-  </si>
-  <si>
-    <t>DiagnosticReport</t>
-  </si>
-  <si>
-    <t>Goal</t>
-  </si>
-  <si>
-    <t>MedicationRequest</t>
-  </si>
-  <si>
-    <t>Procedure</t>
-  </si>
-  <si>
-    <t>Observation</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-diagnosticreport-lab</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-diagnosticreport-note</t>
-  </si>
-  <si>
     <t>!EXAMPLE CATEGORY SEARCH</t>
   </si>
   <si>
@@ -413,21 +371,9 @@
     <t>support searching a patient based on contact information such as phone number or email address</t>
   </si>
   <si>
-    <t>CarePlan</t>
-  </si>
-  <si>
     <t>!EXAMPLE STATUS SEARCH</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careplan</t>
-  </si>
-  <si>
-    <t>CareTeam</t>
-  </si>
-  <si>
-    <t>Device</t>
-  </si>
-  <si>
     <t>Organization</t>
   </si>
   <si>
@@ -437,12 +383,6 @@
     <t>PractitionerRole</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-smokingstatus</t>
-  </si>
-  <si>
-    <t>!DocumentReference</t>
-  </si>
-  <si>
     <t>fixed_kv</t>
   </si>
   <si>
@@ -450,12 +390,6 @@
   </si>
   <si>
     <t>should_include</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-vitalsigns</t>
-  </si>
-  <si>
-    <t>!Observation</t>
   </si>
   <si>
     <t>conf_Organization</t>
@@ -513,12 +447,6 @@
 1. A server **SHALL** reject any unauthorized requests by returning an `HTTP 401` unauthorized response code.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-lab</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-implantable-device</t>
-  </si>
-  <si>
     <t>doc</t>
   </si>
   <si>
@@ -532,9 +460,6 @@
   </si>
   <si>
     <t>history-system</t>
-  </si>
-  <si>
-    <t>!MedicationStatement</t>
   </si>
   <si>
     <t>fhirVersion</t>
@@ -724,53 +649,57 @@
     <t>service-date</t>
   </si>
   <si>
+    <t>provider</t>
+  </si>
+  <si>
+    <t>care-team</t>
+  </si>
+  <si>
+    <t>insurer</t>
+  </si>
+  <si>
+    <t>coverage</t>
+  </si>
+  <si>
+    <t>Practitioner MarkDown Documentation is here</t>
+  </si>
+  <si>
+    <t>Coverage MarkDown Documentation is here</t>
+  </si>
+  <si>
+    <t>PractitionerRole MarkDown Documentation is here</t>
+  </si>
+  <si>
+    <t>Organization MarkDown Documentation is here</t>
+  </si>
+  <si>
+    <t>Patient MarkDown Documentation is here</t>
+  </si>
+  <si>
+    <t>ExplanationOfBenefit:provider,ExplanationOfBenefit:care-team,ExplanationOfBenefit:coverage,ExplanationOfBenefit:location,ExplanationOfBenefit:insurer</t>
+  </si>
+  <si>
+    <t>!ExplanationOfBenefit</t>
+  </si>
+  <si>
     <t>http://hl7.org/fhir/us/carin-bb/StructureDefinition/CARIN-BB-ExplanationOfBenefit-Inpatient-Facility,
 http://hl7.org/fhir/us/carin-bb/StructureDefinition/CARIN-BB-ExplanationOfBenefit-outpatient-Facility,
 http://hl7.org/fhir/us/carin-bb/StructureDefinition/CARIN-BB-ExplanationOfBenefit-Pharmacy,
-http://hl7.org/fhir/us/carin-bb/StructureDefinition/CARIN-BB-ExplanationOfBenefit-Professional-NonClinician, CARIN-BB-Coverage, CARIN-BB-Patient, CARIN-BB-Practitioner, CARIN-BB-PractitionerRole, CARIN-BB-Organization</t>
-  </si>
-  <si>
-    <t>provider</t>
-  </si>
-  <si>
-    <t>care-team</t>
-  </si>
-  <si>
-    <t>insurer</t>
-  </si>
-  <si>
-    <t>coverage</t>
-  </si>
-  <si>
-    <t>ExplanationOfBeneffit MarkDown Documentation is here</t>
-  </si>
-  <si>
-    <t>Practitioner MarkDown Documentation is here</t>
-  </si>
-  <si>
-    <t>Coverage MarkDown Documentation is here</t>
-  </si>
-  <si>
-    <t>PractitionerRole MarkDown Documentation is here</t>
-  </si>
-  <si>
-    <t>Organization MarkDown Documentation is here</t>
-  </si>
-  <si>
-    <t>Patient MarkDown Documentation is here</t>
-  </si>
-  <si>
-    <t>ExplanationOfBenefit:provider,ExplanationOfBenefit:care-team,ExplanationOfBenefit:coverage,ExplanationOfBenefit:location,ExplanationOfBenefit:insurer</t>
-  </si>
-  <si>
-    <t>!ExplanationOfBenefit</t>
+http://hl7.org/fhir/us/carin-bb/StructureDefinition/CARIN-BB-ExplanationOfBenefit-Professional-NonClinician, CARIN-BB-Coverage, CARIN-BB-Patient, CARIN-BB-Practitioner, CARIN-BB-PractitionerRole</t>
+  </si>
+  <si>
+    <t>The EOB Resource is the focal Consumer-Directed Payer Data Exchange (CDPDE) Resource. Several Reference Resources are defined directly/indirectly from the EOB: Coverage, Patient, Organization (Payer ID), Practioner, Organization (Facility), PractionerRole, Location.
+The Coverage Reference Resource SHALL be returned with data that was effective as of the date of service of the claim; for example, the data will reflect the employer name in effect at that time. However, for other reference resources, payers MAY decide to provide either the data that was in effect as of the date of service or the current data. All reference resources within the EOB will have meta.lastUpdated flagged as must support. Payers SHALL provide the last time the data was updated or the date of creation in the payers system of record, whichever comes last. Apps will use the meta.lastUpdated values to determine if the reference resources are as of the current date or date of service.</t>
+  </si>
+  <si>
+    <t>PractitionerRole:organization, PractitionerRole:practitioner</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -918,6 +847,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF323130"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -956,7 +891,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -993,6 +928,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1010,9 +946,10 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
@@ -1350,90 +1287,90 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>141</v>
+        <v>116</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>142</v>
+        <v>117</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>161</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>143</v>
+        <v>118</v>
       </c>
       <c r="B4" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>146</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>145</v>
+        <v>120</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>150</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>151</v>
+        <v>126</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>155</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>151</v>
+        <v>126</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>156</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>152</v>
+        <v>127</v>
       </c>
       <c r="B9" t="s">
-        <v>157</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>153</v>
+        <v>128</v>
       </c>
       <c r="B10" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>154</v>
+        <v>129</v>
       </c>
       <c r="B11" t="s">
-        <v>159</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>160</v>
+        <v>135</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>162</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -1446,10 +1383,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:P84"/>
+  <dimension ref="A1:P83"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:J84"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1468,1260 +1405,463 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="D1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>74</v>
-      </c>
       <c r="G1" s="4" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" s="1" t="str">
-        <f t="shared" ref="C2:C39" si="0">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B2)</f>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
-      </c>
-      <c r="D2"/>
-      <c r="E2"/>
-      <c r="F2"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="82" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="C2" s="30"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
-      </c>
-      <c r="D3"/>
+      <c r="C3" s="30"/>
       <c r="E3"/>
       <c r="F3"/>
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C4" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
-      </c>
-      <c r="D4"/>
+      <c r="C4" s="30"/>
       <c r="E4"/>
       <c r="F4"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
-      </c>
-      <c r="D5"/>
+      <c r="C5" s="30"/>
       <c r="E5"/>
       <c r="F5"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
-      </c>
-      <c r="D6"/>
+      <c r="C6" s="30"/>
       <c r="E6"/>
       <c r="F6"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C7" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
-      </c>
-      <c r="D7"/>
+      <c r="C7" s="30"/>
       <c r="E7"/>
       <c r="F7"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C8" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
-      </c>
-      <c r="D8"/>
+      <c r="C8" s="30"/>
       <c r="E8"/>
       <c r="F8"/>
+      <c r="I8" s="5"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C9" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
-      </c>
-      <c r="D9"/>
+      <c r="C9" s="30"/>
       <c r="E9"/>
       <c r="F9"/>
+      <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C10" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
-      </c>
-      <c r="D10"/>
+      <c r="C10" s="30"/>
       <c r="E10"/>
       <c r="F10"/>
       <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>79</v>
-      </c>
-      <c r="C11" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
-      </c>
-      <c r="D11"/>
+      <c r="C11" s="30"/>
       <c r="E11"/>
       <c r="F11"/>
-      <c r="H11" s="5"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>79</v>
-      </c>
-      <c r="C12" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
-      </c>
-      <c r="D12"/>
+      <c r="C12" s="30"/>
       <c r="E12"/>
       <c r="F12"/>
+      <c r="H12" s="5"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
-      </c>
-      <c r="D13"/>
-      <c r="E13"/>
-      <c r="F13"/>
-      <c r="H13" s="5"/>
+    <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C14" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
-      </c>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C15" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
-      </c>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
-      </c>
+      <c r="I16" s="5"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C17" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
-      </c>
-      <c r="I17" s="5"/>
+    <row r="17" spans="8:10" x14ac:dyDescent="0.2">
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
-      </c>
+    <row r="18" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C19" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
-      </c>
-      <c r="H19" s="5"/>
+    <row r="19" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
-        <v>21</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C20" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
-      </c>
-      <c r="I20" s="5"/>
+    <row r="20" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
-        <v>22</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C21" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
-      </c>
+    <row r="21" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H21" s="5"/>
       <c r="J21" s="5"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
-        <v>23</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C22" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
-      </c>
+    <row r="22" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
-        <v>24</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C23" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
-      </c>
+    <row r="23" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
     </row>
-    <row r="24" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
-        <v>25</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C24" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
-      </c>
+    <row r="24" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
     </row>
-    <row r="25" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
-        <v>26</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C25" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
-      </c>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
+    <row r="25" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
-        <v>27</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C26" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
-      </c>
+    <row r="26" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
-        <v>28</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C27" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
-      </c>
+    <row r="27" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J27" s="5"/>
     </row>
-    <row r="28" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
-        <v>29</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C28" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
-      </c>
+    <row r="28" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
       <c r="J28" s="5"/>
     </row>
-    <row r="29" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
-        <v>30</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
-      </c>
+    <row r="29" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
     </row>
-    <row r="30" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
-        <v>31</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C30" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
-      </c>
+    <row r="30" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
     </row>
-    <row r="31" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="1">
-        <v>32</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C31" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
-      </c>
+    <row r="31" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
     </row>
-    <row r="32" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="1">
-        <v>33</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C32" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
-      </c>
+    <row r="32" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
     </row>
-    <row r="33" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="1">
-        <v>36</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C33" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
-      </c>
+    <row r="33" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
     </row>
-    <row r="34" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="1">
-        <v>37</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C34" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
-      </c>
+    <row r="34" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
     </row>
-    <row r="35" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="1">
-        <v>38</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C35" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
-      </c>
+    <row r="35" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
     </row>
-    <row r="36" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="1">
-        <v>39</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C36" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
-      </c>
+    <row r="36" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
     </row>
-    <row r="37" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="1">
-        <v>42</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C37" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-allergyintolerance</v>
-      </c>
+    <row r="37" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
     </row>
-    <row r="38" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="1">
-        <v>45</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C38" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-immunization</v>
-      </c>
+    <row r="38" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
     </row>
-    <row r="39" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="1">
-        <v>46</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C39" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-immunization</v>
-      </c>
+    <row r="39" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
     </row>
-    <row r="40" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="1">
-        <v>49</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>90</v>
-      </c>
+    <row r="40" spans="3:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="H40" s="5"/>
-      <c r="I40" s="5"/>
+      <c r="I40" s="7"/>
       <c r="J40" s="5"/>
     </row>
-    <row r="41" spans="1:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" s="1">
-        <v>50</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>90</v>
-      </c>
+    <row r="41" spans="3:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="H41" s="5"/>
       <c r="I41" s="7"/>
       <c r="J41" s="5"/>
     </row>
-    <row r="42" spans="1:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="1">
-        <v>51</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>90</v>
-      </c>
+    <row r="42" spans="3:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="H42" s="5"/>
       <c r="I42" s="7"/>
       <c r="J42" s="5"/>
     </row>
-    <row r="43" spans="1:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" s="1">
-        <v>52</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>90</v>
-      </c>
+    <row r="43" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H43" s="5"/>
-      <c r="I43" s="7"/>
+      <c r="I43" s="5"/>
       <c r="J43" s="5"/>
     </row>
-    <row r="44" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="1">
-        <v>53</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>90</v>
-      </c>
+    <row r="44" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C44" s="9"/>
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
     </row>
-    <row r="45" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="1">
-        <v>56</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>91</v>
-      </c>
+    <row r="45" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C45" s="9"/>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
       <c r="J45" s="5"/>
     </row>
-    <row r="46" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="1">
-        <v>57</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>91</v>
-      </c>
+    <row r="46" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C46" s="9"/>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
     </row>
-    <row r="47" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="1">
-        <v>58</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>91</v>
-      </c>
+    <row r="47" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C47" s="9"/>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
     </row>
-    <row r="48" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="1">
-        <v>59</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>91</v>
-      </c>
+    <row r="48" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C48" s="9"/>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
       <c r="J48" s="5"/>
     </row>
-    <row r="49" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="1">
-        <v>60</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>91</v>
-      </c>
+    <row r="49" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
       <c r="J49" s="5"/>
     </row>
-    <row r="50" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="1">
-        <v>63</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C50" s="1" t="str">
-        <f t="shared" ref="C50:C60" si="1">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B50)</f>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
-      </c>
+    <row r="50" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H50" s="5"/>
       <c r="I50" s="5"/>
       <c r="J50" s="5"/>
     </row>
-    <row r="51" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="1">
-        <v>64</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C51" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
-      </c>
+    <row r="51" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
       <c r="J51" s="5"/>
     </row>
-    <row r="52" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="1">
-        <v>67</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C52" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
-      </c>
+    <row r="52" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H52" s="5"/>
       <c r="I52" s="5"/>
       <c r="J52" s="5"/>
     </row>
-    <row r="53" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="1">
-        <v>68</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C53" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
-      </c>
+    <row r="53" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
     </row>
-    <row r="54" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="1">
-        <v>69</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C54" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
-      </c>
+    <row r="54" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
       <c r="J54" s="5"/>
     </row>
-    <row r="55" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="1">
-        <v>70</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C55" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
-      </c>
+    <row r="55" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
       <c r="J55" s="5"/>
     </row>
-    <row r="56" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="1">
-        <v>73</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C56" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationstatement</v>
-      </c>
+    <row r="56" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H56" s="5"/>
       <c r="I56" s="5"/>
       <c r="J56" s="5"/>
     </row>
-    <row r="57" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="1">
-        <v>74</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C57" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationstatement</v>
-      </c>
+    <row r="57" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
       <c r="J57" s="5"/>
     </row>
-    <row r="58" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="1">
-        <v>75</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C58" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
-      </c>
+    <row r="58" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H58" s="5"/>
       <c r="I58" s="5"/>
       <c r="J58" s="5"/>
     </row>
-    <row r="59" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="1">
-        <v>76</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C59" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
-      </c>
+    <row r="59" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H59" s="5"/>
       <c r="I59" s="5"/>
       <c r="J59" s="5"/>
     </row>
-    <row r="60" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="1">
-        <v>77</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C60" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
-      </c>
+    <row r="60" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H60" s="5"/>
       <c r="I60" s="5"/>
       <c r="J60" s="5"/>
     </row>
-    <row r="61" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="1">
-        <v>80</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>130</v>
-      </c>
+    <row r="61" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
       <c r="J61" s="5"/>
     </row>
-    <row r="62" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="1">
-        <v>81</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>130</v>
-      </c>
+    <row r="62" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H62" s="5"/>
       <c r="I62" s="5"/>
       <c r="J62" s="5"/>
     </row>
-    <row r="63" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="1">
-        <v>82</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>130</v>
-      </c>
+    <row r="63" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C63" s="9"/>
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>
       <c r="J63" s="5"/>
     </row>
-    <row r="64" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="1">
-        <v>83</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C64" s="9" t="s">
-        <v>130</v>
-      </c>
+    <row r="64" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C64" s="9"/>
       <c r="H64" s="5"/>
       <c r="I64" s="5"/>
       <c r="J64" s="5"/>
     </row>
-    <row r="65" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="1">
-        <v>84</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>130</v>
-      </c>
+    <row r="65" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H65" s="5"/>
       <c r="I65" s="5"/>
       <c r="J65" s="5"/>
     </row>
-    <row r="66" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="1">
-        <v>85</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>130</v>
-      </c>
+    <row r="66" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C66" s="9"/>
       <c r="H66" s="5"/>
       <c r="I66" s="5"/>
       <c r="J66" s="5"/>
     </row>
-    <row r="67" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="1">
-        <v>88</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C67" s="9" t="s">
-        <v>99</v>
-      </c>
+    <row r="67" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C67" s="9"/>
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>
       <c r="J67" s="5"/>
     </row>
-    <row r="68" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="1">
-        <v>89</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C68" s="9" t="s">
-        <v>99</v>
-      </c>
+    <row r="68" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C68" s="9"/>
       <c r="H68" s="5"/>
       <c r="I68" s="5"/>
       <c r="J68" s="5"/>
     </row>
-    <row r="69" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="1">
-        <v>90</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C69" s="9" t="s">
-        <v>99</v>
-      </c>
+    <row r="69" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C69" s="9"/>
       <c r="H69" s="5"/>
       <c r="I69" s="5"/>
       <c r="J69" s="5"/>
     </row>
-    <row r="70" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="1">
-        <v>91</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C70" s="9" t="s">
-        <v>99</v>
-      </c>
+    <row r="70" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H70" s="5"/>
       <c r="I70" s="5"/>
       <c r="J70" s="5"/>
     </row>
-    <row r="71" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="1">
-        <v>94</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C71" s="1" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B71)</f>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
-      </c>
+    <row r="71" spans="3:16" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="C71" s="8"/>
       <c r="H71" s="5"/>
       <c r="I71" s="5"/>
       <c r="J71" s="5"/>
     </row>
-    <row r="72" spans="1:16" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A72" s="1">
-        <v>97</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C72" s="8" t="s">
-        <v>105</v>
-      </c>
+    <row r="72" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H72" s="5"/>
       <c r="I72" s="5"/>
       <c r="J72" s="5"/>
     </row>
-    <row r="73" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="1">
-        <v>100</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>110</v>
-      </c>
+    <row r="73" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H73" s="5"/>
       <c r="I73" s="5"/>
       <c r="J73" s="5"/>
     </row>
-    <row r="74" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="1">
-        <v>101</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>110</v>
-      </c>
+    <row r="74" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H74" s="5"/>
       <c r="I74" s="5"/>
       <c r="J74" s="5"/>
     </row>
-    <row r="75" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="1">
-        <v>102</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>110</v>
-      </c>
+    <row r="75" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H75" s="5"/>
       <c r="I75" s="5"/>
       <c r="J75" s="5"/>
     </row>
-    <row r="76" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="1">
-        <v>103</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>110</v>
-      </c>
+    <row r="76" spans="3:16" x14ac:dyDescent="0.2">
       <c r="H76" s="5"/>
       <c r="I76" s="5"/>
       <c r="J76" s="5"/>
-    </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A77" s="1">
-        <v>104</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>110</v>
-      </c>
+      <c r="K76" s="1"/>
+      <c r="L76" s="1"/>
+      <c r="M76" s="1"/>
+      <c r="N76" s="1"/>
+      <c r="O76" s="1"/>
+      <c r="P76" s="1"/>
+    </row>
+    <row r="77" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H77" s="5"/>
       <c r="I77" s="5"/>
       <c r="J77" s="5"/>
-      <c r="K77" s="1"/>
-      <c r="L77" s="1"/>
-      <c r="M77" s="1"/>
-      <c r="N77" s="1"/>
-      <c r="O77" s="1"/>
-      <c r="P77" s="1"/>
-    </row>
-    <row r="78" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="1">
-        <v>107</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C78" s="1" t="str">
-        <f t="shared" ref="C78:C83" si="2">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B78)</f>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
-      </c>
+    </row>
+    <row r="78" spans="3:16" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H78" s="5"/>
       <c r="I78" s="5"/>
       <c r="J78" s="5"/>
     </row>
-    <row r="79" spans="1:16" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="1">
-        <v>108</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C79" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!documentreference</v>
-      </c>
+    <row r="79" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H79" s="5"/>
       <c r="I79" s="5"/>
       <c r="J79" s="5"/>
     </row>
-    <row r="80" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="1">
-        <v>109</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C80" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
-      </c>
+    <row r="80" spans="3:16" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H80" s="5"/>
-      <c r="I80" s="5"/>
+      <c r="I80" s="7"/>
       <c r="J80" s="5"/>
     </row>
-    <row r="81" spans="1:10" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="1">
-        <v>110</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C81" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
-      </c>
+    <row r="81" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H81" s="5"/>
-      <c r="I81" s="7"/>
+      <c r="I81" s="5"/>
       <c r="J81" s="5"/>
     </row>
-    <row r="82" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="1">
-        <v>111</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C82" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
-      </c>
+    <row r="82" spans="8:10" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H82" s="5"/>
       <c r="I82" s="5"/>
       <c r="J82" s="5"/>
     </row>
-    <row r="83" spans="1:10" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="1">
-        <v>112</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C83" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
-      </c>
+    <row r="83" spans="8:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="H83" s="5"/>
       <c r="I83" s="5"/>
       <c r="J83" s="5"/>
     </row>
-    <row r="84" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="1">
-        <v>115</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="H84" s="5"/>
-      <c r="I84" s="5"/>
-      <c r="J84" s="5"/>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J128">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J127">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2756,23 +1896,23 @@
         <v>2</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>139</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>138</v>
+        <v>113</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>147</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -2780,7 +1920,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -2788,7 +1928,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -2804,7 +1944,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>185</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2812,7 +1952,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -2835,10 +1975,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2862,152 +2002,152 @@
     <col min="4" max="4" width="16.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="26" customFormat="1" ht="26" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:6" s="27" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A1" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="27" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
-        <v>170</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>174</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>165</v>
+      <c r="A2" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>140</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
-        <v>171</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>177</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="24" t="s">
-        <v>165</v>
+      <c r="A3" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>140</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
-        <v>173</v>
-      </c>
-      <c r="B4" s="24" t="s">
-        <v>176</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="24" t="s">
-        <v>165</v>
+      <c r="A4" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>140</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
-        <v>175</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>178</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="24" t="s">
-        <v>165</v>
+      <c r="A5" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>140</v>
       </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
-        <v>172</v>
-      </c>
-      <c r="B6" s="24" t="s">
-        <v>179</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>164</v>
+      <c r="A6" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>139</v>
       </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
-        <v>169</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>180</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>104</v>
+      <c r="A7" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>86</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
-        <v>168</v>
-      </c>
-      <c r="B8" s="24" t="s">
-        <v>181</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>102</v>
+      <c r="A8" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>84</v>
       </c>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="B9" s="24" t="s">
-        <v>182</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="24" t="s">
-        <v>103</v>
+      <c r="A9" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>85</v>
       </c>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
-        <v>166</v>
-      </c>
-      <c r="B10" s="24" t="s">
-        <v>183</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="24" t="s">
-        <v>23</v>
+      <c r="A10" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -3024,7 +2164,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3056,61 +2196,61 @@
         <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="F1" t="s">
         <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="H1" t="s">
         <v>18</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>119</v>
+        <v>97</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="R1" t="s">
         <v>19</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="T1" s="11" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="U1" s="11" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="V1" s="11" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
       <c r="W1" s="11" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="X1" t="s">
         <v>20</v>
@@ -3118,13 +2258,13 @@
     </row>
     <row r="2" spans="1:24" ht="18" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>164</v>
+        <v>139</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>202</v>
+        <v>175</v>
       </c>
       <c r="D2"/>
       <c r="F2"/>
@@ -3138,15 +2278,15 @@
       <c r="W2" s="20"/>
       <c r="X2"/>
     </row>
-    <row r="3" spans="1:24" ht="81" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="351" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>165</v>
+        <v>140</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>200</v>
+        <v>182</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>21</v>
@@ -3155,19 +2295,19 @@
         <v>13</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>206</v>
+        <v>179</v>
       </c>
       <c r="W3" s="20"/>
     </row>
     <row r="4" spans="1:24" ht="17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>201</v>
+        <v>174</v>
       </c>
       <c r="R4" s="1" t="s">
         <v>21</v>
@@ -3180,13 +2320,13 @@
     </row>
     <row r="5" spans="1:24" ht="33" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>203</v>
+        <v>176</v>
       </c>
       <c r="R5" s="1" t="s">
         <v>21</v>
@@ -3194,18 +2334,21 @@
       <c r="S5" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="T5" s="33" t="s">
+        <v>183</v>
+      </c>
       <c r="W5" s="20"/>
       <c r="X5"/>
     </row>
     <row r="6" spans="1:24" ht="17" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>204</v>
+        <v>177</v>
       </c>
       <c r="R6" s="1" t="s">
         <v>21</v>
@@ -3218,13 +2361,13 @@
     </row>
     <row r="7" spans="1:24" ht="17" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>205</v>
+        <v>178</v>
       </c>
       <c r="R7" s="1" t="s">
         <v>21</v>
@@ -3276,16 +2419,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
         <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E1" t="s">
         <v>7</v>
@@ -3307,7 +2450,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3323,30 +2466,30 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>187</v>
+        <v>162</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>188</v>
+        <v>163</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C2" s="1"/>
       <c r="E2" s="1"/>
@@ -3355,7 +2498,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>13</v>
@@ -3363,22 +2506,13 @@
       <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
@@ -3401,25 +2535,25 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1"/>
       <c r="E6" s="1"/>
@@ -3428,7 +2562,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C7" s="1"/>
       <c r="E7" s="1"/>
@@ -3437,7 +2571,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C8" s="1"/>
       <c r="E8" s="1"/>
@@ -3446,7 +2580,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C9" s="1"/>
       <c r="E9" s="1"/>
@@ -3455,7 +2589,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C10" s="1"/>
       <c r="E10" s="1"/>
@@ -3489,39 +2623,39 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>132</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>133</v>
+        <v>109</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>134</v>
+        <v>110</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>135</v>
+        <v>111</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="2"/>
@@ -3535,11 +2669,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AB37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B16" sqref="B16:B19"/>
+      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3549,7 +2683,7 @@
     <col min="3" max="3" width="33.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" customWidth="1"/>
-    <col min="6" max="6" width="73.83203125" style="30" customWidth="1"/>
+    <col min="6" max="6" width="75.5" style="31" customWidth="1"/>
     <col min="8" max="8" width="14.33203125" customWidth="1"/>
     <col min="9" max="9" width="23.5" customWidth="1"/>
     <col min="10" max="10" width="36.1640625" style="1" bestFit="1" customWidth="1"/>
@@ -3575,88 +2709,88 @@
   <sheetData>
     <row r="1" spans="1:28" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1" s="27" t="s">
+      <c r="G1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="H1" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>14</v>
       </c>
       <c r="J1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="U1" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="W1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>56</v>
       </c>
       <c r="Y1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="Z1" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="AA1" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AB1" s="6" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="13" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
@@ -3664,39 +2798,39 @@
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E2" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="F2" s="28" t="str">
+      <c r="F2" s="29" t="str">
         <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B2)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!example category search</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J2" s="13" t="str">
         <f>B2&amp;"."&amp;C2</f>
         <v>!EXAMPLE CATEGORY SEARCH.category</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="Y2" s="14"/>
       <c r="Z2" s="14"/>
@@ -3711,10 +2845,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>13</v>
@@ -3722,28 +2856,28 @@
       <c r="E3" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="F3" s="28" t="str">
+      <c r="F3" s="29" t="str">
         <f t="shared" ref="F3:F8" si="1">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B3)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!example code search</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J3" s="13" t="str">
         <f>B3&amp;"."&amp;C3</f>
         <v>!EXAMPLE CODE SEARCH.code</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M3" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="Y3" s="14"/>
       <c r="Z3" s="14"/>
@@ -3758,10 +2892,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>13</v>
@@ -3769,31 +2903,31 @@
       <c r="E4" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="F4" s="28" t="str">
+      <c r="F4" s="29" t="str">
         <f t="shared" si="1"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!example date search</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J4" s="13" t="str">
         <f>B4&amp;"."&amp;C4</f>
         <v>!EXAMPLE DATE SEARCH.date</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M4" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="N4" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="AA4" s="15"/>
       <c r="AB4" s="13" t="str">
@@ -3806,10 +2940,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>13</v>
@@ -3817,28 +2951,28 @@
       <c r="E5" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="F5" s="28" t="str">
+      <c r="F5" s="29" t="str">
         <f t="shared" si="1"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!example patient search</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J5" s="13" t="str">
         <f>B5&amp;"."&amp;C5</f>
         <v>!EXAMPLE PATIENT SEARCH.patient</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M5" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="Y5" s="13" t="str">
         <f>"support searching for all "&amp;LOWER(B5)&amp;"s for a patient"</f>
@@ -3859,10 +2993,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>13</v>
@@ -3870,28 +3004,28 @@
       <c r="E6" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="F6" s="28" t="str">
+      <c r="F6" s="29" t="str">
         <f t="shared" si="1"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!example status search</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J6" s="13" t="str">
         <f t="shared" ref="J6" si="2">B6&amp;"."&amp;C6</f>
         <v>!EXAMPLE STATUS SEARCH.status</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M6" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="Y6" s="14"/>
       <c r="Z6" s="14"/>
@@ -3906,10 +3040,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>13</v>
@@ -3917,31 +3051,31 @@
       <c r="E7" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="F7" s="28" t="str">
+      <c r="F7" s="29" t="str">
         <f t="shared" si="1"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!patient</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J7" s="13" t="str">
         <f t="shared" ref="J7:J8" si="4">B7&amp;"."&amp;C7</f>
         <v>!Patient.address</v>
       </c>
       <c r="K7" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M7" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="Y7" s="13" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="Z7" s="14"/>
       <c r="AA7" s="15"/>
@@ -3955,10 +3089,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="13" t="s">
         <v>67</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>69</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>13</v>
@@ -3966,31 +3100,31 @@
       <c r="E8" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="F8" s="28" t="str">
+      <c r="F8" s="29" t="str">
         <f t="shared" si="1"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!patient</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J8" s="13" t="str">
         <f t="shared" si="4"/>
         <v>!Patient.telecom</v>
       </c>
       <c r="K8" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M8" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="Y8" s="13" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="AA8" s="15"/>
       <c r="AB8" s="13" t="str">
@@ -4003,10 +3137,10 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>165</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>190</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -4014,27 +3148,27 @@
       <c r="E9" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F9" s="29" t="s">
-        <v>195</v>
+      <c r="F9" s="30" t="s">
+        <v>181</v>
       </c>
       <c r="G9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J9" t="str">
         <f>B9&amp;"."&amp;"managingOrganization"</f>
         <v>ExplanationOfBenefit.managingOrganization</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="X9"/>
       <c r="Y9" s="17"/>
@@ -4051,10 +3185,10 @@
         <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>165</v>
+        <v>140</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>13</v>
@@ -4062,27 +3196,27 @@
       <c r="E10" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F10" s="29" t="s">
-        <v>191</v>
+      <c r="F10" s="30" t="s">
+        <v>166</v>
       </c>
       <c r="G10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J10" s="1" t="str">
         <f t="shared" ref="J10:J14" si="6">B10&amp;"."&amp;C10</f>
         <v>ExplanationOfBenefit.patient</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="P10"/>
       <c r="Q10"/>
@@ -4099,16 +3233,16 @@
         <v>SearchParameter-plan-net-explanationofbenefit-patient.html</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="144" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" ht="52" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <f t="shared" ref="A11:A19" si="9">A10+1</f>
+        <f t="shared" ref="A11:A27" si="9">A10+1</f>
         <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>165</v>
+        <v>140</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>193</v>
+        <v>168</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -4116,27 +3250,27 @@
       <c r="E11" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F11" s="31" t="s">
-        <v>195</v>
+      <c r="F11" s="30" t="s">
+        <v>166</v>
       </c>
       <c r="G11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J11" s="1" t="str">
         <f t="shared" si="6"/>
         <v>ExplanationOfBenefit._lastUpdated</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="O11"/>
       <c r="X11"/>
@@ -4157,7 +3291,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>165</v>
+        <v>140</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>14</v>
@@ -4168,27 +3302,27 @@
       <c r="E12" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F12" s="29" t="s">
-        <v>191</v>
+      <c r="F12" s="30" t="s">
+        <v>166</v>
       </c>
       <c r="G12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J12" s="1" t="str">
         <f>B12&amp;"."&amp;"provided_by"</f>
         <v>ExplanationOfBenefit.provided_by</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="Y12" s="17" t="str">
         <f t="shared" si="7"/>
@@ -4206,10 +3340,10 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>165</v>
+        <v>140</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>192</v>
+        <v>167</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -4217,27 +3351,27 @@
       <c r="E13" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F13" s="29" t="s">
-        <v>191</v>
+      <c r="F13" s="30" t="s">
+        <v>166</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J13" s="1" t="str">
         <f t="shared" ref="J13" si="10">B13&amp;"."&amp;C13</f>
         <v>ExplanationOfBenefit.identifier</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="Y13" s="17" t="str">
         <f t="shared" ref="Y13" si="11">"Support searching for a "&amp; B12 &amp;" by its " &amp; C13</f>
@@ -4255,10 +3389,10 @@
         <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>165</v>
+        <v>140</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>194</v>
+        <v>169</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -4266,27 +3400,27 @@
       <c r="E14" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F14" s="29" t="s">
-        <v>191</v>
+      <c r="F14" s="30" t="s">
+        <v>166</v>
       </c>
       <c r="G14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J14" s="1" t="str">
         <f t="shared" si="6"/>
         <v>ExplanationOfBenefit.service-date</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="Y14" s="17" t="str">
         <f>"Support searching for a "&amp; B12 &amp;" by its " &amp; C14</f>
@@ -4304,10 +3438,10 @@
         <v>7</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>207</v>
+        <v>180</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>196</v>
+        <v>170</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>13</v>
@@ -4315,27 +3449,27 @@
       <c r="E15" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F15" s="29" t="s">
-        <v>191</v>
+      <c r="F15" s="30" t="s">
+        <v>166</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J15" s="1" t="str">
         <f t="shared" ref="J15:J19" si="13">B15&amp;"."&amp;C15</f>
         <v>!ExplanationOfBenefit.provider</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="S15" s="1" t="s">
         <v>13</v>
@@ -4360,10 +3494,10 @@
         <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>207</v>
+        <v>180</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>197</v>
+        <v>171</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -4371,27 +3505,27 @@
       <c r="E16" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F16" s="29" t="s">
-        <v>191</v>
+      <c r="F16" s="30" t="s">
+        <v>166</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J16" s="1" t="str">
         <f t="shared" si="13"/>
         <v>!ExplanationOfBenefit.care-team</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="S16" s="1" t="s">
         <v>13</v>
@@ -4416,10 +3550,10 @@
         <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>207</v>
+        <v>180</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>198</v>
+        <v>172</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -4427,27 +3561,27 @@
       <c r="E17" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F17" s="29" t="s">
-        <v>191</v>
+      <c r="F17" s="30" t="s">
+        <v>166</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J17" s="1" t="str">
         <f t="shared" si="13"/>
         <v>!ExplanationOfBenefit.insurer</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="S17" s="1" t="s">
         <v>13</v>
@@ -4472,10 +3606,10 @@
         <v>10</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>207</v>
+        <v>180</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>13</v>
@@ -4483,27 +3617,27 @@
       <c r="E18" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F18" s="29" t="s">
-        <v>191</v>
+      <c r="F18" s="30" t="s">
+        <v>166</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J18" s="1" t="str">
         <f t="shared" si="13"/>
         <v>!ExplanationOfBenefit.location</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="S18" s="1" t="s">
         <v>13</v>
@@ -4528,10 +3662,10 @@
         <v>11</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>207</v>
+        <v>180</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>199</v>
+        <v>173</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -4539,27 +3673,27 @@
       <c r="E19" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F19" s="29" t="s">
-        <v>191</v>
+      <c r="F19" s="30" t="s">
+        <v>166</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J19" s="1" t="str">
         <f t="shared" si="13"/>
         <v>!ExplanationOfBenefit.coverage</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="S19" s="1" t="s">
         <v>13</v>
@@ -4579,63 +3713,355 @@
       </c>
     </row>
     <row r="20" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
+      <c r="A20" s="1">
+        <f t="shared" si="9"/>
+        <v>12</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J20" s="1" t="str">
+        <f t="shared" ref="J20:J23" si="16">B20&amp;"."&amp;"managingOrganization"</f>
+        <v>Coverage.managingOrganization</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="Y20" s="17"/>
       <c r="AB20" s="1"/>
     </row>
     <row r="21" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
+      <c r="A21" s="1">
+        <f t="shared" si="9"/>
+        <v>13</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F21" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J21" s="1" t="str">
+        <f t="shared" si="16"/>
+        <v>Practitioner.managingOrganization</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="Y21" s="17"/>
       <c r="AB21" s="1"/>
     </row>
     <row r="22" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
+      <c r="A22" s="1">
+        <f t="shared" si="9"/>
+        <v>14</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J22" s="1" t="str">
+        <f t="shared" si="16"/>
+        <v>PractitionerRole.managingOrganization</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="Y22" s="17"/>
       <c r="AB22" s="1"/>
     </row>
     <row r="23" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
+      <c r="A23" s="1">
+        <f t="shared" si="9"/>
+        <v>15</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F23" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J23" s="1" t="str">
+        <f t="shared" si="16"/>
+        <v>Organization.managingOrganization</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S23" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="Y23" s="17"/>
       <c r="AB23" s="1"/>
     </row>
-    <row r="24" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
+    <row r="24" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <f t="shared" si="9"/>
+        <v>16</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F24" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J24" s="1" t="str">
+        <f t="shared" ref="J24:J27" si="17">B24&amp;"."&amp;"managingOrganization"</f>
+        <v>Coverage.managingOrganization</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="Y24" s="17"/>
-      <c r="AB24" s="1"/>
-    </row>
-    <row r="25" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
+      <c r="AA24" s="2"/>
+    </row>
+    <row r="25" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <f t="shared" si="9"/>
+        <v>17</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F25" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J25" s="1" t="str">
+        <f t="shared" si="17"/>
+        <v>Practitioner.managingOrganization</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="Y25" s="17"/>
-      <c r="AB25" s="1"/>
-    </row>
-    <row r="26" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
+      <c r="AA25" s="2"/>
+    </row>
+    <row r="26" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <f t="shared" si="9"/>
+        <v>18</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F26" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J26" s="1" t="str">
+        <f t="shared" si="17"/>
+        <v>PractitionerRole.managingOrganization</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="Y26" s="17"/>
-      <c r="AB26" s="1"/>
-    </row>
-    <row r="27" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
+      <c r="AA26" s="2"/>
+    </row>
+    <row r="27" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <f t="shared" si="9"/>
+        <v>19</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F27" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J27" s="1" t="str">
+        <f t="shared" si="17"/>
+        <v>Organization.managingOrganization</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="Y27" s="17"/>
-      <c r="AB27" s="1"/>
+      <c r="AA27" s="2"/>
     </row>
     <row r="28" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F28" s="30"/>
+      <c r="F28" s="31"/>
       <c r="Y28" s="17"/>
       <c r="AA28" s="2"/>
     </row>
@@ -4707,8 +4133,18 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:AA19">
     <sortCondition ref="B1"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="F23" r:id="rId1" xr:uid="{7DB736E8-A50D-E540-B3A4-68714BE32FDB}"/>
+    <hyperlink ref="F20" r:id="rId2" xr:uid="{A7BD924E-2AE3-E944-BA4C-5FB895D21DE3}"/>
+    <hyperlink ref="F21" r:id="rId3" xr:uid="{FEA219A9-76C2-864D-BD61-058F3F4F7417}"/>
+    <hyperlink ref="F22" r:id="rId4" xr:uid="{35EC8646-19B4-5440-996B-480BDD42ABE6}"/>
+    <hyperlink ref="F27" r:id="rId5" xr:uid="{1A044EA7-8217-0A47-813C-EA43B50F824D}"/>
+    <hyperlink ref="F24" r:id="rId6" xr:uid="{3E81C577-5F18-AB45-A3C9-255BBBDE9DCC}"/>
+    <hyperlink ref="F25" r:id="rId7" xr:uid="{8865180D-D514-1C4E-AF22-84F2B7DBF539}"/>
+    <hyperlink ref="F26" r:id="rId8" xr:uid="{003AAAA6-C254-5F4C-B4B3-1C05AA1B40D4}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId9"/>
+  <legacyDrawing r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added config to skip rest.interactions section
</commit_message>
<xml_diff>
--- a/CapStatement/temp_source_spreadsheets/carin-bb-server.xlsx
+++ b/CapStatement/temp_source_spreadsheets/carin-bb-server.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skravitz/git-alt/MyNotebooks/CapStatement/temp_source_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C490518C-DD07-2040-8A3C-BEA28046C9B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6195E525-520C-A84C-997C-E5CD6E62FAF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4280" yWindow="2780" windowWidth="64520" windowHeight="25180" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4280" yWindow="2780" windowWidth="64520" windowHeight="25180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="185">
   <si>
     <t>Element</t>
   </si>
@@ -378,9 +378,6 @@
   </si>
   <si>
     <t>Practitioner</t>
-  </si>
-  <si>
-    <t>PractitionerRole</t>
   </si>
   <si>
     <t>fixed_kv</t>
@@ -552,9 +549,6 @@
     <t>http://hl7.org/fhir/us/carin-bb/StructureDefinition/CARIN-BB-Organization</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/carin-bb/StructureDefinition/CARIN-BB-PractitionerRole</t>
-  </si>
-  <si>
     <t>http://hl7.org/fhir/us/carin-bb/StructureDefinition/CARIN-BB-ExplanationOfBenefit-Inpatient-Facility</t>
   </si>
   <si>
@@ -582,9 +576,6 @@
     <t>CARIN-BB-Coverage</t>
   </si>
   <si>
-    <t>CARIN-BB-PractitionerRole</t>
-  </si>
-  <si>
     <t>CARIN-BB-Organization</t>
   </si>
   <si>
@@ -630,26 +621,7 @@
     <t>coverage</t>
   </si>
   <si>
-    <t>Practitioner MarkDown Documentation is here</t>
-  </si>
-  <si>
-    <t>Coverage MarkDown Documentation is here</t>
-  </si>
-  <si>
-    <t>PractitionerRole MarkDown Documentation is here</t>
-  </si>
-  <si>
-    <t>Organization MarkDown Documentation is here</t>
-  </si>
-  <si>
-    <t>Patient MarkDown Documentation is here</t>
-  </si>
-  <si>
     <t>!ExplanationOfBenefit</t>
-  </si>
-  <si>
-    <t>The EOB Resource is the focal Consumer-Directed Payer Data Exchange (CDPDE) Resource. Several Reference Resources are defined directly/indirectly from the EOB: Coverage, Patient, Organization (Payer ID), Practioner, Organization (Facility), PractionerRole, Location.
-The Coverage Reference Resource SHALL be returned with data that was effective as of the date of service of the claim; for example, the data will reflect the employer name in effect at that time. However, for other reference resources, payers MAY decide to provide either the data that was in effect as of the date of service or the current data. All reference resources within the EOB will have meta.lastUpdated flagged as must support. Payers SHALL provide the last time the data was updated or the date of creation in the payers system of record, whichever comes last. Apps will use the meta.lastUpdated values to determine if the reference resources are as of the current date or date of service.</t>
   </si>
   <si>
     <t>doc_ExplanationOfBenefit</t>
@@ -669,13 +641,39 @@
     <t>http://hl7.org/fhir/us/carin-bb/ImplementationGuide/hl7.fhir.us.carin-bb</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/carin-bb/StructureDefinition/CARIN-BB-ExplanationOfBenefit-Inpatient-Facility,
+    <t>facility</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/carin-bb/StructureDefinition/CARIN-BB-ExplanationOfBenefit-Outpatient-Facility</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/carin-bb/StructureDefinition/CARIN-BB-ExplanationOfBenefit</t>
+  </si>
+  <si>
+    <t>CARIN-BB-ExplanationOfBenefit</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/carin-bb/StructureDefinition/CARIN-BB-ExplanationOfBenefit,http://hl7.org/fhir/us/carin-bb/StructureDefinition/CARIN-BB-ExplanationOfBenefit-Inpatient-Facility,
 http://hl7.org/fhir/us/carin-bb/StructureDefinition/CARIN-BB-ExplanationOfBenefit-Outpatient-Facility,
 http://hl7.org/fhir/us/carin-bb/StructureDefinition/CARIN-BB-ExplanationOfBenefit-Pharmacy,
 http://hl7.org/fhir/us/carin-bb/StructureDefinition/CARIN-BB-ExplanationOfBenefit-Professional-NonClinician</t>
   </si>
   <si>
-    <t>PractitionerRole:organization,PractitionerRole:practitioner</t>
+    <t>The EOB Resource is the focal Consumer-Directed Payer Data Exchange (CDPDE) Resource. Several Reference Resources are defined directly/indirectly from the EOB: Coverage, Patient, Organization (Payer ID), Practioner, Organization (Facility), PractionerRole, Location.
+The Coverage Reference Resource SHALL be returned with data that was effective as of the date of service of the claim; for example, the data will reflect the employer name in effect at that time. However, for other reference resources, payers MAY decide to provide either the data that was in effect as of the date of service or the current data. All reference resources within the EOB will have meta.lastUpdated flagged as must support. Payers SHALL provide the last time the data was updated or the date of creation in the payers system of record, whichever comes last. Apps will use the meta.lastUpdated values to determine if the reference resources are as of the current date or date of service.
+When an EOB references another resource (e.g., Patient or Practitioner), the reference may be versioned or versionless. Payers SHALL use versioned references whenever they maintain point-in-time data (data that was effective as of the date of service or date of admission on the claim), but MAY use versionless references when they do not maintain versioned data. Clients MAY request referenced resources as part of an EOB search (by supplying the _include parameter) or directly using read or vread. Payers SHALL support both approaches, and SHALL return the same content for referenced resources in either case.</t>
+  </si>
+  <si>
+    <t>Coverage:payor</t>
+  </si>
+  <si>
+    <t>!Coverage</t>
+  </si>
+  <si>
+    <t>ExplanationOfBenefit:provider,ExplanationOfBenefit:care-team,ExplanationOfBenefit:coverage,ExplanationOfBenefit:insurer,ExplanationOfBenefit:*</t>
   </si>
   <si>
     <t xml:space="preserve">The Carin-bb  Server **SHALL**:
@@ -687,23 +685,17 @@
    - (Status 403): insufficient scope
    - (Status 404): unknown resource
    - (Status 410): deleted resource.
-1. Support json source formats for all Plan-Net interactions.
+1. Support json source formats for all Carin-bbinteractions.
 1. Identify the CARIN-BB  profiles supported as part of the FHIR `meta.profile` attribute for each instance.
-The Plan-Net  Server **SHOULD**:
-1. Support xml source formats for all Plan-Net  interactions.
+The Carin-bb  Server **SHOULD**:
+1. Support xml source formats for all Carin-bb interactions.
 </t>
   </si>
   <si>
-    <t>facility</t>
-  </si>
-  <si>
-    <t>ExplanationOfBenefit:provider,ExplanationOfBenefit:care-team,ExplanationOfBenefit:coverage,ExplanationOfBenefit:facility,ExplanationOfBenefit:insurer</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/carin-bb/StructureDefinition/CARIN-BB-ExplanationOfBenefit-Outpatient-Facility</t>
-  </si>
-  <si>
-    <t>N</t>
+    <t>skip rest interaction section</t>
+  </si>
+  <si>
+    <t>rest</t>
   </si>
 </sst>
 </file>
@@ -859,8 +851,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="16"/>
-      <color rgb="FF323130"/>
+      <sz val="15"/>
+      <color rgb="FF201F1E"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
@@ -957,10 +949,10 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
@@ -1277,10 +1269,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C527BFB-CCF4-354D-B696-43330F2FE9C6}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1297,96 +1289,107 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>123</v>
+      <c r="A2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>135</v>
+        <v>114</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B4" t="s">
-        <v>122</v>
+        <v>115</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>120</v>
+        <v>116</v>
+      </c>
+      <c r="B5" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>119</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>129</v>
+        <v>118</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>130</v>
+        <v>124</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>126</v>
-      </c>
-      <c r="B9" t="s">
-        <v>131</v>
+      <c r="A9" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>134</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>136</v>
+        <v>127</v>
+      </c>
+      <c r="B12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>133</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{F32193F9-BCC1-B84B-9F7E-EBC5551BAE49}"/>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{F32193F9-BCC1-B84B-9F7E-EBC5551BAE49}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1434,7 +1437,7 @@
         <v>72</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>3</v>
@@ -1885,7 +1888,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1907,7 +1910,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1915,15 +1918,15 @@
         <v>62</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1931,7 +1934,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1939,7 +1942,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1955,7 +1958,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1963,7 +1966,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1979,7 +1982,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2002,7 +2005,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView zoomScale="105" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2027,72 +2030,71 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
-        <v>144</v>
+    <row r="2" spans="1:6" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>175</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>147</v>
+        <v>176</v>
       </c>
       <c r="C2" s="25" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="F2" s="1"/>
+        <v>138</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>186</v>
+      <c r="A3" s="23" t="s">
+        <v>142</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C3" s="25" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
-        <v>146</v>
+      <c r="A4" s="12" t="s">
+        <v>173</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C4" s="25" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C5" s="25" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C6" s="25" t="s">
         <v>13</v>
@@ -2107,22 +2109,22 @@
         <v>143</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C7" s="25" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>86</v>
+        <v>137</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C8" s="25" t="s">
         <v>13</v>
@@ -2134,10 +2136,10 @@
     </row>
     <row r="9" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C9" s="25" t="s">
         <v>13</v>
@@ -2149,10 +2151,10 @@
     </row>
     <row r="10" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C10" s="25" t="s">
         <v>13</v>
@@ -2163,22 +2165,23 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{DB5855A9-36F9-B146-BC04-BF373D3B96B6}"/>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{DB5855A9-36F9-B146-BC04-BF373D3B96B6}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{354343EB-05FC-BE4A-A5C5-AB9258320A2C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:X43"/>
+  <dimension ref="A1:X42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="B17" sqref="B16:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2210,75 +2213,72 @@
         <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F1" t="s">
         <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H1" t="s">
         <v>18</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="R1" t="s">
         <v>19</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="T1" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="U1" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="11" t="s">
-        <v>89</v>
-      </c>
       <c r="V1" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="W1" s="11" t="s">
         <v>95</v>
-      </c>
-      <c r="W1" s="11" t="s">
-        <v>96</v>
       </c>
       <c r="X1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="18" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" ht="21" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>170</v>
       </c>
       <c r="D2"/>
       <c r="F2"/>
@@ -2288,19 +2288,22 @@
       <c r="S2" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="T2" s="32" t="s">
+        <v>179</v>
+      </c>
       <c r="V2" s="20"/>
       <c r="W2" s="20"/>
       <c r="X2"/>
     </row>
-    <row r="3" spans="1:24" ht="351" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>139</v>
+    <row r="3" spans="1:24" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>138</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>21</v>
@@ -2309,20 +2312,17 @@
         <v>13</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="W3" s="20"/>
     </row>
-    <row r="4" spans="1:24" ht="17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>169</v>
-      </c>
       <c r="R4" s="1" t="s">
         <v>21</v>
       </c>
@@ -2332,15 +2332,12 @@
       <c r="V4" s="20"/>
       <c r="W4" s="20"/>
     </row>
-    <row r="5" spans="1:24" ht="33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" ht="16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="R5" s="1" t="s">
         <v>21</v>
@@ -2348,21 +2345,15 @@
       <c r="S5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="T5" s="33" t="s">
-        <v>182</v>
-      </c>
+      <c r="V5" s="20"/>
       <c r="W5" s="20"/>
-      <c r="X5"/>
-    </row>
-    <row r="6" spans="1:24" ht="17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:24" ht="16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>84</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>172</v>
       </c>
       <c r="R6" s="1" t="s">
         <v>21</v>
@@ -2370,44 +2361,25 @@
       <c r="S6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="V6" s="20"/>
       <c r="W6" s="20"/>
     </row>
-    <row r="7" spans="1:24" ht="17" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="W7" s="20"/>
+    <row r="7" spans="1:24" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7"/>
     </row>
     <row r="8" spans="1:24" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8"/>
     </row>
-    <row r="9" spans="1:24" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9"/>
-    </row>
-    <row r="40" spans="20:23" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T40" s="21"/>
-      <c r="V40" s="21"/>
-      <c r="W40" s="21"/>
-    </row>
-    <row r="43" spans="20:23" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="W43" s="21"/>
+    <row r="39" spans="20:23" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T39" s="21"/>
+      <c r="V39" s="21"/>
+      <c r="W39" s="21"/>
+    </row>
+    <row r="42" spans="20:23" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W42" s="21"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A7">
-    <sortCondition ref="A2:A7"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A6">
+    <sortCondition ref="A2:A6"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2484,28 +2456,28 @@
         <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -2534,7 +2506,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -2546,7 +2518,7 @@
         <v>13</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>13</v>
@@ -2567,7 +2539,7 @@
         <v>63</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>63</v>
@@ -2637,7 +2609,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2654,43 +2626,35 @@
         <v>25</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>30</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="B2" s="1"/>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>30</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="B3" s="1"/>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>30</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="B4" s="1"/>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>30</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="B5" s="1"/>
       <c r="C5" s="2"/>
     </row>
   </sheetData>
@@ -2700,13 +2664,13 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:AB37"/>
+  <dimension ref="A1:AB30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="6" ySplit="1" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B30" sqref="B30"/>
+      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2802,10 +2766,10 @@
         <v>52</v>
       </c>
       <c r="U1" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="V1" s="4" t="s">
         <v>88</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>89</v>
       </c>
       <c r="W1" s="4" t="s">
         <v>53</v>
@@ -2968,7 +2932,7 @@
         <v>SearchParameter-us-core-!example date search-date.html</v>
       </c>
     </row>
-    <row r="5" spans="1:28" s="13" customFormat="1" ht="31" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" s="13" customFormat="1" ht="61" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
         <v>4</v>
       </c>
@@ -3165,15 +3129,15 @@
         <v>SearchParameter-us-core-!patient-telecom.html</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="52" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" ht="65" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -3182,13 +3146,13 @@
         <v>1</v>
       </c>
       <c r="F9" s="30" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="G9" t="s">
         <v>57</v>
       </c>
       <c r="H9" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="I9" t="s">
         <v>58</v>
@@ -3208,17 +3172,17 @@
       <c r="Z9" s="5"/>
       <c r="AA9" s="10"/>
       <c r="AB9" s="1" t="str">
-        <f t="shared" ref="AB9:AB19" si="6">"SearchParameter-carin-bb-"&amp;LOWER((B9)&amp;"-"&amp;C9&amp;".html")</f>
+        <f t="shared" ref="AB9" si="6">"SearchParameter-carin-bb-"&amp;LOWER((B9)&amp;"-"&amp;C9&amp;".html")</f>
         <v>SearchParameter-carin-bb-explanationofbenefit-_id.html</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="52" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" ht="65" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <f>A9+1</f>
         <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>68</v>
@@ -3230,7 +3194,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="30" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="G10" t="s">
         <v>57</v>
@@ -3266,16 +3230,16 @@
         <v>SearchParameter-carin-bb-explanationofbenefit-patient.html</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="52" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" ht="65" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <f t="shared" ref="A11:A27" si="9">A10+1</f>
+        <f t="shared" ref="A11:A19" si="9">A10+1</f>
         <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -3284,13 +3248,13 @@
         <v>1</v>
       </c>
       <c r="F11" s="30" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="G11" t="s">
         <v>57</v>
       </c>
       <c r="H11" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>64</v>
@@ -3314,17 +3278,17 @@
       <c r="Z11" s="5"/>
       <c r="AA11" s="10"/>
       <c r="AB11" s="1" t="str">
-        <f t="shared" ref="AB11:AB27" si="10">"SearchParameter-carin-bb-"&amp;LOWER((B11)&amp;"-"&amp;C11&amp;".html")</f>
+        <f t="shared" ref="AB11:AB19" si="10">"SearchParameter-carin-bb-"&amp;LOWER((B11)&amp;"-"&amp;C11&amp;".html")</f>
         <v>SearchParameter-carin-bb-explanationofbenefit-_lastupdated.html</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="52" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" ht="65" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>14</v>
@@ -3336,7 +3300,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="30" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="G12" t="s">
         <v>57</v>
@@ -3367,16 +3331,16 @@
         <v>SearchParameter-carin-bb-explanationofbenefit-type.html</v>
       </c>
     </row>
-    <row r="13" spans="1:28" s="1" customFormat="1" ht="52" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" s="1" customFormat="1" ht="65" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -3385,7 +3349,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="30" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>57</v>
@@ -3416,16 +3380,16 @@
         <v>SearchParameter-carin-bb-explanationofbenefit-identifier.html</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="52" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" ht="65" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -3434,7 +3398,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="30" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="G14" t="s">
         <v>57</v>
@@ -3465,16 +3429,16 @@
         <v>SearchParameter-carin-bb-explanationofbenefit-service-date.html</v>
       </c>
     </row>
-    <row r="15" spans="1:28" s="1" customFormat="1" ht="52" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" s="1" customFormat="1" ht="65" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>13</v>
@@ -3483,7 +3447,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="30" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>57</v>
@@ -3521,16 +3485,16 @@
         <v>SearchParameter-carin-bb-!explanationofbenefit-provider.html</v>
       </c>
     </row>
-    <row r="16" spans="1:28" s="1" customFormat="1" ht="52" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" s="1" customFormat="1" ht="65" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
@@ -3539,7 +3503,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="30" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>57</v>
@@ -3577,16 +3541,16 @@
         <v>SearchParameter-carin-bb-!explanationofbenefit-care-team.html</v>
       </c>
     </row>
-    <row r="17" spans="1:28" s="1" customFormat="1" ht="52" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:28" s="1" customFormat="1" ht="65" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -3595,7 +3559,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="30" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>57</v>
@@ -3633,16 +3597,16 @@
         <v>SearchParameter-carin-bb-!explanationofbenefit-insurer.html</v>
       </c>
     </row>
-    <row r="18" spans="1:28" s="1" customFormat="1" ht="52" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:28" s="1" customFormat="1" ht="65" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>13</v>
@@ -3651,7 +3615,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="30" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>57</v>
@@ -3689,16 +3653,16 @@
         <v>SearchParameter-carin-bb-!explanationofbenefit-facility.html</v>
       </c>
     </row>
-    <row r="19" spans="1:28" s="1" customFormat="1" ht="52" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" s="1" customFormat="1" ht="65" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <f t="shared" si="9"/>
         <v>11</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -3707,7 +3671,7 @@
         <v>1</v>
       </c>
       <c r="F19" s="30" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>57</v>
@@ -3747,14 +3711,14 @@
     </row>
     <row r="20" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <f t="shared" si="9"/>
+        <f>A19+1</f>
         <v>12</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>138</v>
+        <v>180</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -3763,20 +3727,20 @@
         <v>1</v>
       </c>
       <c r="F20" s="22" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>57</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>58</v>
       </c>
       <c r="J20" s="1" t="str">
-        <f t="shared" ref="J20:J23" si="15">B20&amp;"."&amp;"managingOrganization"</f>
-        <v>Coverage.managingOrganization</v>
+        <f>B20&amp;"."&amp;"managingOrganization"</f>
+        <v>!Coverage.managingOrganization</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>57</v>
@@ -3789,342 +3753,63 @@
       </c>
       <c r="Y20" s="17"/>
       <c r="AB20" s="1" t="str">
-        <f t="shared" si="10"/>
-        <v>SearchParameter-carin-bb-coverage-_id.html</v>
-      </c>
-    </row>
-    <row r="21" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
-        <f t="shared" si="9"/>
-        <v>13</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F21" s="22" t="s">
-        <v>141</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="J21" s="1" t="str">
-        <f t="shared" si="15"/>
-        <v>Practitioner.managingOrganization</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="S21" s="1" t="s">
-        <v>13</v>
-      </c>
+        <f>"SearchParameter-carin-bb-"&amp;LOWER((B20)&amp;"-"&amp;C20&amp;".html")</f>
+        <v>SearchParameter-carin-bb-!coverage-_id.html</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F21" s="31"/>
       <c r="Y21" s="17"/>
-      <c r="AB21" s="1" t="str">
-        <f t="shared" si="10"/>
-        <v>SearchParameter-carin-bb-practitioner-_id.html</v>
-      </c>
+      <c r="AA21" s="2"/>
     </row>
     <row r="22" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
-        <f t="shared" si="9"/>
-        <v>14</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F22" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="J22" s="1" t="str">
-        <f t="shared" si="15"/>
-        <v>PractitionerRole.managingOrganization</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="S22" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
       <c r="Y22" s="17"/>
-      <c r="AB22" s="1" t="str">
-        <f t="shared" si="10"/>
-        <v>SearchParameter-carin-bb-practitionerrole-_id.html</v>
-      </c>
+      <c r="AB22" s="1"/>
     </row>
     <row r="23" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
-        <f t="shared" si="9"/>
-        <v>15</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F23" s="32" t="s">
-        <v>142</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="J23" s="1" t="str">
-        <f t="shared" si="15"/>
-        <v>Organization.managingOrganization</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="S23" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
       <c r="Y23" s="17"/>
-      <c r="AB23" s="1" t="str">
-        <f t="shared" si="10"/>
-        <v>SearchParameter-carin-bb-organization-_id.html</v>
-      </c>
-    </row>
-    <row r="24" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
-        <f t="shared" si="9"/>
-        <v>16</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F24" s="22" t="s">
-        <v>145</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J24" s="1" t="str">
-        <f t="shared" ref="J24:J27" si="16">B24&amp;"."&amp;"managingOrganization"</f>
-        <v>Coverage.managingOrganization</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>57</v>
-      </c>
+      <c r="AB23" s="1"/>
+    </row>
+    <row r="24" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
       <c r="Y24" s="17"/>
-      <c r="AA24" s="2"/>
-      <c r="AB24" s="1" t="str">
-        <f t="shared" si="10"/>
-        <v>SearchParameter-carin-bb-coverage-_lastupdated.html</v>
-      </c>
-    </row>
-    <row r="25" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
-        <f t="shared" si="9"/>
-        <v>17</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F25" s="22" t="s">
-        <v>141</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J25" s="1" t="str">
-        <f t="shared" si="16"/>
-        <v>Practitioner.managingOrganization</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="M25" s="1" t="s">
-        <v>57</v>
-      </c>
+      <c r="AB24" s="1"/>
+    </row>
+    <row r="25" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
       <c r="Y25" s="17"/>
-      <c r="AA25" s="2"/>
-      <c r="AB25" s="1" t="str">
-        <f t="shared" si="10"/>
-        <v>SearchParameter-carin-bb-practitioner-_lastupdated.html</v>
-      </c>
-    </row>
-    <row r="26" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
-        <f t="shared" si="9"/>
-        <v>18</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F26" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J26" s="1" t="str">
-        <f t="shared" si="16"/>
-        <v>PractitionerRole.managingOrganization</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>57</v>
-      </c>
+      <c r="AB25" s="1"/>
+    </row>
+    <row r="26" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
       <c r="Y26" s="17"/>
-      <c r="AA26" s="2"/>
-      <c r="AB26" s="1" t="str">
-        <f t="shared" si="10"/>
-        <v>SearchParameter-carin-bb-practitionerrole-_lastupdated.html</v>
-      </c>
-    </row>
-    <row r="27" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
-        <f t="shared" si="9"/>
-        <v>19</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E27" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F27" s="32" t="s">
-        <v>142</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J27" s="1" t="str">
-        <f t="shared" si="16"/>
-        <v>Organization.managingOrganization</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="M27" s="1" t="s">
-        <v>57</v>
-      </c>
+      <c r="AB26" s="1"/>
+    </row>
+    <row r="27" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
       <c r="Y27" s="17"/>
-      <c r="AA27" s="2"/>
-      <c r="AB27" s="1" t="str">
-        <f t="shared" si="10"/>
-        <v>SearchParameter-carin-bb-organization-_lastupdated.html</v>
-      </c>
-    </row>
-    <row r="28" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F28" s="31"/>
+      <c r="AB27" s="1"/>
+    </row>
+    <row r="28" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
       <c r="Y28" s="17"/>
-      <c r="AA28" s="2"/>
+      <c r="AB28" s="1"/>
     </row>
     <row r="29" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G29" s="1"/>
@@ -4140,72 +3825,16 @@
       <c r="Y30" s="17"/>
       <c r="AB30" s="1"/>
     </row>
-    <row r="31" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="Y31" s="17"/>
-      <c r="AB31" s="1"/>
-    </row>
-    <row r="32" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="Y32" s="17"/>
-      <c r="AB32" s="1"/>
-    </row>
-    <row r="33" spans="7:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="Y33" s="17"/>
-      <c r="AB33" s="1"/>
-    </row>
-    <row r="34" spans="7:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="Y34" s="17"/>
-      <c r="AB34" s="1"/>
-    </row>
-    <row r="35" spans="7:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="Y35" s="17"/>
-      <c r="AB35" s="1"/>
-    </row>
-    <row r="36" spans="7:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="Y36" s="17"/>
-      <c r="AB36" s="1"/>
-    </row>
-    <row r="37" spans="7:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="Y37" s="17"/>
-      <c r="AB37" s="1"/>
-    </row>
   </sheetData>
   <autoFilter ref="A1:AB19" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:AA19">
     <sortCondition ref="B1"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="F23" r:id="rId1" xr:uid="{7DB736E8-A50D-E540-B3A4-68714BE32FDB}"/>
-    <hyperlink ref="F20" r:id="rId2" xr:uid="{A7BD924E-2AE3-E944-BA4C-5FB895D21DE3}"/>
-    <hyperlink ref="F21" r:id="rId3" xr:uid="{FEA219A9-76C2-864D-BD61-058F3F4F7417}"/>
-    <hyperlink ref="F22" r:id="rId4" xr:uid="{35EC8646-19B4-5440-996B-480BDD42ABE6}"/>
-    <hyperlink ref="F27" r:id="rId5" xr:uid="{1A044EA7-8217-0A47-813C-EA43B50F824D}"/>
-    <hyperlink ref="F24" r:id="rId6" xr:uid="{3E81C577-5F18-AB45-A3C9-255BBBDE9DCC}"/>
-    <hyperlink ref="F25" r:id="rId7" xr:uid="{8865180D-D514-1C4E-AF22-84F2B7DBF539}"/>
-    <hyperlink ref="F26" r:id="rId8" xr:uid="{003AAAA6-C254-5F4C-B4B3-1C05AA1B40D4}"/>
+    <hyperlink ref="F20" r:id="rId1" xr:uid="{A7BD924E-2AE3-E944-BA4C-5FB895D21DE3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId9"/>
-  <legacyDrawing r:id="rId10"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>